<commit_message>
26 Apr 2024 - Codes were modified to support one group of questions in question bank.
</commit_message>
<xml_diff>
--- a/static/candidates.xlsx
+++ b/static/candidates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_web/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_web/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57EC8B5-816E-1647-93EE-91C94CBABBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B308E9EB-22FD-2F45-98A7-690EDF460ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="2960" windowWidth="27640" windowHeight="16940" xr2:uid="{33DC2F0A-A837-CC48-AC78-A8FB66671071}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>cand_no</t>
   </si>
@@ -140,9 +140,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC3D66E-995A-6B4C-88A0-411F10AD1979}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,7 +510,7 @@
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1111</v>
       </c>
       <c r="C2" t="s">
@@ -529,7 +530,7 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>1111</v>
       </c>
       <c r="C3" t="s">
@@ -549,7 +550,7 @@
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>1111</v>
       </c>
       <c r="C4" t="s">
@@ -569,7 +570,7 @@
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1112</v>
       </c>
       <c r="C5" t="s">
@@ -589,7 +590,7 @@
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>1112</v>
       </c>
       <c r="C6" t="s">
@@ -609,7 +610,7 @@
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>1113</v>
       </c>
       <c r="C7" t="s">
@@ -629,7 +630,7 @@
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>1113</v>
       </c>
       <c r="C8" t="s">
@@ -649,7 +650,7 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>1113</v>
       </c>
       <c r="C9" t="s">
@@ -669,7 +670,7 @@
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>1114</v>
       </c>
       <c r="C10" t="s">
@@ -689,7 +690,7 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>1114</v>
       </c>
       <c r="C11" t="s">
@@ -703,6 +704,46 @@
       </c>
       <c r="F11" s="1">
         <v>65432109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2222</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1">
+        <v>65432109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2222</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1">
+        <v>98765432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>